<commit_message>
updated raw data with spawn/brood data
</commit_message>
<xml_diff>
--- a/data/data_table_factors - data.xlsx
+++ b/data/data_table_factors - data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2610" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2803" uniqueCount="167">
   <si>
     <t>paper</t>
   </si>
@@ -514,13 +514,13 @@
     <t>Monstrea faveolata</t>
   </si>
   <si>
-    <t>Miscelanous Items - airstone and tubing</t>
+    <t>Large birth size does not reduce negative latent effects of harsh environments across life stages in two coral species</t>
   </si>
   <si>
-    <t>Hartman</t>
+    <t>Hartman, Marhaver, Chamberland, Sandin and Vermeij</t>
   </si>
   <si>
-    <t>A. humlis</t>
+    <t>Agaricia humlis</t>
   </si>
 </sst>
 </file>
@@ -1004,10 +1004,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1331,14 +1330,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A322" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG328" sqref="AG328"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E333" sqref="E333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="27.1796875" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.35">
@@ -5468,6 +5468,9 @@
       <c r="D69">
         <v>17</v>
       </c>
+      <c r="E69" t="s">
+        <v>36</v>
+      </c>
       <c r="F69" t="s">
         <v>64</v>
       </c>
@@ -5521,6 +5524,9 @@
       <c r="D70">
         <v>17</v>
       </c>
+      <c r="E70" t="s">
+        <v>36</v>
+      </c>
       <c r="F70" t="s">
         <v>64</v>
       </c>
@@ -5574,6 +5580,9 @@
       <c r="D71">
         <v>17</v>
       </c>
+      <c r="E71" t="s">
+        <v>36</v>
+      </c>
       <c r="F71" t="s">
         <v>64</v>
       </c>
@@ -5627,6 +5636,9 @@
       <c r="D72">
         <v>17</v>
       </c>
+      <c r="E72" t="s">
+        <v>36</v>
+      </c>
       <c r="F72" t="s">
         <v>64</v>
       </c>
@@ -5680,6 +5692,9 @@
       <c r="D73">
         <v>17</v>
       </c>
+      <c r="E73" t="s">
+        <v>36</v>
+      </c>
       <c r="F73" t="s">
         <v>64</v>
       </c>
@@ -6013,6 +6028,9 @@
       <c r="D79">
         <v>17</v>
       </c>
+      <c r="E79" t="s">
+        <v>36</v>
+      </c>
       <c r="F79" t="s">
         <v>64</v>
       </c>
@@ -6066,6 +6084,9 @@
       <c r="D80">
         <v>17</v>
       </c>
+      <c r="E80" t="s">
+        <v>36</v>
+      </c>
       <c r="F80" t="s">
         <v>64</v>
       </c>
@@ -6119,6 +6140,9 @@
       <c r="D81">
         <v>17</v>
       </c>
+      <c r="E81" t="s">
+        <v>36</v>
+      </c>
       <c r="F81" t="s">
         <v>64</v>
       </c>
@@ -6172,6 +6196,9 @@
       <c r="D82">
         <v>17</v>
       </c>
+      <c r="E82" t="s">
+        <v>36</v>
+      </c>
       <c r="F82" t="s">
         <v>64</v>
       </c>
@@ -6225,6 +6252,9 @@
       <c r="D83">
         <v>17</v>
       </c>
+      <c r="E83" t="s">
+        <v>36</v>
+      </c>
       <c r="F83" t="s">
         <v>64</v>
       </c>
@@ -7549,6 +7579,9 @@
       <c r="D106">
         <v>24</v>
       </c>
+      <c r="E106" t="s">
+        <v>36</v>
+      </c>
       <c r="F106" t="s">
         <v>37</v>
       </c>
@@ -7605,6 +7638,9 @@
       <c r="D107">
         <v>25</v>
       </c>
+      <c r="E107" t="s">
+        <v>36</v>
+      </c>
       <c r="F107" t="s">
         <v>37</v>
       </c>
@@ -7661,6 +7697,9 @@
       <c r="D108">
         <v>25</v>
       </c>
+      <c r="E108" t="s">
+        <v>36</v>
+      </c>
       <c r="F108" t="s">
         <v>37</v>
       </c>
@@ -7717,6 +7756,9 @@
       <c r="D109">
         <v>25</v>
       </c>
+      <c r="E109" t="s">
+        <v>36</v>
+      </c>
       <c r="F109" t="s">
         <v>37</v>
       </c>
@@ -7773,6 +7815,9 @@
       <c r="D110">
         <v>25</v>
       </c>
+      <c r="E110" t="s">
+        <v>36</v>
+      </c>
       <c r="F110" t="s">
         <v>37</v>
       </c>
@@ -12007,6 +12052,9 @@
       <c r="D184">
         <v>39</v>
       </c>
+      <c r="E184" t="s">
+        <v>36</v>
+      </c>
       <c r="F184" t="s">
         <v>54</v>
       </c>
@@ -12054,6 +12102,9 @@
       <c r="D185">
         <v>39</v>
       </c>
+      <c r="E185" t="s">
+        <v>36</v>
+      </c>
       <c r="F185" t="s">
         <v>54</v>
       </c>
@@ -12101,6 +12152,9 @@
       <c r="D186">
         <v>39</v>
       </c>
+      <c r="E186" t="s">
+        <v>36</v>
+      </c>
       <c r="F186" t="s">
         <v>54</v>
       </c>
@@ -12148,6 +12202,9 @@
       <c r="D187">
         <v>39</v>
       </c>
+      <c r="E187" t="s">
+        <v>36</v>
+      </c>
       <c r="F187" t="s">
         <v>54</v>
       </c>
@@ -12195,6 +12252,9 @@
       <c r="D188">
         <v>39</v>
       </c>
+      <c r="E188" t="s">
+        <v>36</v>
+      </c>
       <c r="F188" t="s">
         <v>54</v>
       </c>
@@ -12242,6 +12302,9 @@
       <c r="D189">
         <v>39</v>
       </c>
+      <c r="E189" t="s">
+        <v>36</v>
+      </c>
       <c r="F189" t="s">
         <v>54</v>
       </c>
@@ -12289,6 +12352,9 @@
       <c r="D190">
         <v>40</v>
       </c>
+      <c r="E190" t="s">
+        <v>36</v>
+      </c>
       <c r="F190" t="s">
         <v>54</v>
       </c>
@@ -12333,6 +12399,9 @@
       <c r="D191">
         <v>40</v>
       </c>
+      <c r="E191" t="s">
+        <v>36</v>
+      </c>
       <c r="F191" t="s">
         <v>54</v>
       </c>
@@ -12377,6 +12446,9 @@
       <c r="D192">
         <v>40</v>
       </c>
+      <c r="E192" t="s">
+        <v>36</v>
+      </c>
       <c r="F192" t="s">
         <v>54</v>
       </c>
@@ -12421,6 +12493,9 @@
       <c r="D193">
         <v>41</v>
       </c>
+      <c r="E193" t="s">
+        <v>36</v>
+      </c>
       <c r="F193" t="s">
         <v>54</v>
       </c>
@@ -12465,6 +12540,9 @@
       <c r="D194">
         <v>41</v>
       </c>
+      <c r="E194" t="s">
+        <v>36</v>
+      </c>
       <c r="F194" t="s">
         <v>54</v>
       </c>
@@ -12509,6 +12587,9 @@
       <c r="D195">
         <v>42</v>
       </c>
+      <c r="E195" t="s">
+        <v>36</v>
+      </c>
       <c r="F195" t="s">
         <v>54</v>
       </c>
@@ -12556,6 +12637,9 @@
       <c r="D196">
         <v>42</v>
       </c>
+      <c r="E196" t="s">
+        <v>36</v>
+      </c>
       <c r="F196" t="s">
         <v>54</v>
       </c>
@@ -12603,6 +12687,9 @@
       <c r="D197">
         <v>43</v>
       </c>
+      <c r="E197" t="s">
+        <v>36</v>
+      </c>
       <c r="F197" t="s">
         <v>54</v>
       </c>
@@ -12650,6 +12737,9 @@
       <c r="D198">
         <v>43</v>
       </c>
+      <c r="E198" t="s">
+        <v>36</v>
+      </c>
       <c r="F198" t="s">
         <v>54</v>
       </c>
@@ -12697,6 +12787,9 @@
       <c r="D199">
         <v>44</v>
       </c>
+      <c r="E199" t="s">
+        <v>36</v>
+      </c>
       <c r="F199" t="s">
         <v>37</v>
       </c>
@@ -12744,6 +12837,9 @@
       <c r="D200">
         <v>44</v>
       </c>
+      <c r="E200" t="s">
+        <v>36</v>
+      </c>
       <c r="F200" t="s">
         <v>37</v>
       </c>
@@ -12791,6 +12887,9 @@
       <c r="D201">
         <v>44</v>
       </c>
+      <c r="E201" t="s">
+        <v>36</v>
+      </c>
       <c r="F201" t="s">
         <v>37</v>
       </c>
@@ -12838,6 +12937,9 @@
       <c r="D202">
         <v>45</v>
       </c>
+      <c r="E202" t="s">
+        <v>36</v>
+      </c>
       <c r="F202" t="s">
         <v>54</v>
       </c>
@@ -12888,6 +12990,9 @@
       <c r="D203">
         <v>45</v>
       </c>
+      <c r="E203" t="s">
+        <v>36</v>
+      </c>
       <c r="F203" t="s">
         <v>54</v>
       </c>
@@ -12938,6 +13043,9 @@
       <c r="D204">
         <v>45</v>
       </c>
+      <c r="E204" t="s">
+        <v>36</v>
+      </c>
       <c r="F204" t="s">
         <v>54</v>
       </c>
@@ -12988,6 +13096,9 @@
       <c r="D205">
         <v>45</v>
       </c>
+      <c r="E205" t="s">
+        <v>36</v>
+      </c>
       <c r="F205" t="s">
         <v>54</v>
       </c>
@@ -13038,6 +13149,9 @@
       <c r="D206">
         <v>45</v>
       </c>
+      <c r="E206" t="s">
+        <v>36</v>
+      </c>
       <c r="F206" t="s">
         <v>54</v>
       </c>
@@ -13088,6 +13202,9 @@
       <c r="D207">
         <v>45</v>
       </c>
+      <c r="E207" t="s">
+        <v>36</v>
+      </c>
       <c r="F207" t="s">
         <v>54</v>
       </c>
@@ -13138,6 +13255,9 @@
       <c r="D208">
         <v>46</v>
       </c>
+      <c r="E208" t="s">
+        <v>36</v>
+      </c>
       <c r="F208" t="s">
         <v>54</v>
       </c>
@@ -13182,6 +13302,9 @@
       <c r="D209">
         <v>46</v>
       </c>
+      <c r="E209" t="s">
+        <v>36</v>
+      </c>
       <c r="F209" t="s">
         <v>54</v>
       </c>
@@ -13226,6 +13349,9 @@
       <c r="D210">
         <v>46</v>
       </c>
+      <c r="E210" t="s">
+        <v>36</v>
+      </c>
       <c r="F210" t="s">
         <v>54</v>
       </c>
@@ -13270,6 +13396,9 @@
       <c r="D211">
         <v>46</v>
       </c>
+      <c r="E211" t="s">
+        <v>36</v>
+      </c>
       <c r="F211" t="s">
         <v>54</v>
       </c>
@@ -13314,6 +13443,9 @@
       <c r="D212">
         <v>47</v>
       </c>
+      <c r="E212" t="s">
+        <v>36</v>
+      </c>
       <c r="F212" t="s">
         <v>54</v>
       </c>
@@ -13361,6 +13493,9 @@
       <c r="D213">
         <v>47</v>
       </c>
+      <c r="E213" t="s">
+        <v>36</v>
+      </c>
       <c r="F213" t="s">
         <v>54</v>
       </c>
@@ -13408,6 +13543,9 @@
       <c r="D214">
         <v>47</v>
       </c>
+      <c r="E214" t="s">
+        <v>36</v>
+      </c>
       <c r="F214" t="s">
         <v>54</v>
       </c>
@@ -13455,6 +13593,9 @@
       <c r="D215">
         <v>47</v>
       </c>
+      <c r="E215" t="s">
+        <v>36</v>
+      </c>
       <c r="F215" t="s">
         <v>54</v>
       </c>
@@ -13502,6 +13643,9 @@
       <c r="D216">
         <v>47</v>
       </c>
+      <c r="E216" t="s">
+        <v>36</v>
+      </c>
       <c r="F216" t="s">
         <v>54</v>
       </c>
@@ -13549,6 +13693,9 @@
       <c r="D217">
         <v>47</v>
       </c>
+      <c r="E217" t="s">
+        <v>36</v>
+      </c>
       <c r="F217" t="s">
         <v>54</v>
       </c>
@@ -13596,6 +13743,9 @@
       <c r="D218">
         <v>47</v>
       </c>
+      <c r="E218" t="s">
+        <v>36</v>
+      </c>
       <c r="F218" t="s">
         <v>54</v>
       </c>
@@ -13643,6 +13793,9 @@
       <c r="D219">
         <v>47</v>
       </c>
+      <c r="E219" t="s">
+        <v>36</v>
+      </c>
       <c r="F219" t="s">
         <v>54</v>
       </c>
@@ -13690,6 +13843,9 @@
       <c r="D220">
         <v>47</v>
       </c>
+      <c r="E220" t="s">
+        <v>36</v>
+      </c>
       <c r="F220" t="s">
         <v>54</v>
       </c>
@@ -13737,6 +13893,9 @@
       <c r="D221">
         <v>47</v>
       </c>
+      <c r="E221" t="s">
+        <v>36</v>
+      </c>
       <c r="F221" t="s">
         <v>54</v>
       </c>
@@ -13784,6 +13943,9 @@
       <c r="D222">
         <v>47</v>
       </c>
+      <c r="E222" t="s">
+        <v>36</v>
+      </c>
       <c r="F222" t="s">
         <v>54</v>
       </c>
@@ -13831,6 +13993,9 @@
       <c r="D223">
         <v>47</v>
       </c>
+      <c r="E223" t="s">
+        <v>36</v>
+      </c>
       <c r="F223" t="s">
         <v>54</v>
       </c>
@@ -13878,6 +14043,9 @@
       <c r="D224">
         <v>47</v>
       </c>
+      <c r="E224" t="s">
+        <v>36</v>
+      </c>
       <c r="F224" t="s">
         <v>54</v>
       </c>
@@ -13925,6 +14093,9 @@
       <c r="D225">
         <v>47</v>
       </c>
+      <c r="E225" t="s">
+        <v>36</v>
+      </c>
       <c r="F225" t="s">
         <v>54</v>
       </c>
@@ -13972,6 +14143,9 @@
       <c r="D226">
         <v>47</v>
       </c>
+      <c r="E226" t="s">
+        <v>36</v>
+      </c>
       <c r="F226" t="s">
         <v>54</v>
       </c>
@@ -14019,6 +14193,9 @@
       <c r="D227">
         <v>47</v>
       </c>
+      <c r="E227" t="s">
+        <v>36</v>
+      </c>
       <c r="F227" t="s">
         <v>54</v>
       </c>
@@ -14066,6 +14243,9 @@
       <c r="D228">
         <v>48</v>
       </c>
+      <c r="E228" t="s">
+        <v>36</v>
+      </c>
       <c r="F228" t="s">
         <v>54</v>
       </c>
@@ -14113,6 +14293,9 @@
       <c r="D229">
         <v>48</v>
       </c>
+      <c r="E229" t="s">
+        <v>36</v>
+      </c>
       <c r="F229" t="s">
         <v>54</v>
       </c>
@@ -14160,6 +14343,9 @@
       <c r="D230">
         <v>48</v>
       </c>
+      <c r="E230" t="s">
+        <v>36</v>
+      </c>
       <c r="F230" t="s">
         <v>54</v>
       </c>
@@ -14207,6 +14393,9 @@
       <c r="D231">
         <v>48</v>
       </c>
+      <c r="E231" t="s">
+        <v>36</v>
+      </c>
       <c r="F231" t="s">
         <v>54</v>
       </c>
@@ -14254,6 +14443,9 @@
       <c r="D232">
         <v>48</v>
       </c>
+      <c r="E232" t="s">
+        <v>36</v>
+      </c>
       <c r="F232" t="s">
         <v>54</v>
       </c>
@@ -14301,6 +14493,9 @@
       <c r="D233">
         <v>48</v>
       </c>
+      <c r="E233" t="s">
+        <v>36</v>
+      </c>
       <c r="F233" t="s">
         <v>54</v>
       </c>
@@ -14348,6 +14543,9 @@
       <c r="D234">
         <v>48</v>
       </c>
+      <c r="E234" t="s">
+        <v>36</v>
+      </c>
       <c r="F234" t="s">
         <v>54</v>
       </c>
@@ -14395,6 +14593,9 @@
       <c r="D235">
         <v>48</v>
       </c>
+      <c r="E235" t="s">
+        <v>36</v>
+      </c>
       <c r="F235" t="s">
         <v>54</v>
       </c>
@@ -14442,6 +14643,9 @@
       <c r="D236">
         <v>48</v>
       </c>
+      <c r="E236" t="s">
+        <v>36</v>
+      </c>
       <c r="F236" t="s">
         <v>54</v>
       </c>
@@ -14489,6 +14693,9 @@
       <c r="D237">
         <v>48</v>
       </c>
+      <c r="E237" t="s">
+        <v>36</v>
+      </c>
       <c r="F237" t="s">
         <v>54</v>
       </c>
@@ -14536,6 +14743,9 @@
       <c r="D238">
         <v>48</v>
       </c>
+      <c r="E238" t="s">
+        <v>36</v>
+      </c>
       <c r="F238" t="s">
         <v>54</v>
       </c>
@@ -14583,6 +14793,9 @@
       <c r="D239">
         <v>48</v>
       </c>
+      <c r="E239" t="s">
+        <v>36</v>
+      </c>
       <c r="F239" t="s">
         <v>54</v>
       </c>
@@ -14630,6 +14843,9 @@
       <c r="D240">
         <v>48</v>
       </c>
+      <c r="E240" t="s">
+        <v>36</v>
+      </c>
       <c r="F240" t="s">
         <v>54</v>
       </c>
@@ -14677,6 +14893,9 @@
       <c r="D241">
         <v>49</v>
       </c>
+      <c r="E241" t="s">
+        <v>36</v>
+      </c>
       <c r="F241" t="s">
         <v>37</v>
       </c>
@@ -14721,6 +14940,9 @@
       <c r="D242">
         <v>49</v>
       </c>
+      <c r="E242" t="s">
+        <v>36</v>
+      </c>
       <c r="F242" t="s">
         <v>37</v>
       </c>
@@ -14765,6 +14987,9 @@
       <c r="D243">
         <v>49</v>
       </c>
+      <c r="E243" t="s">
+        <v>36</v>
+      </c>
       <c r="F243" t="s">
         <v>37</v>
       </c>
@@ -14809,6 +15034,9 @@
       <c r="D244">
         <v>49</v>
       </c>
+      <c r="E244" t="s">
+        <v>36</v>
+      </c>
       <c r="F244" t="s">
         <v>37</v>
       </c>
@@ -14853,6 +15081,9 @@
       <c r="D245">
         <v>49</v>
       </c>
+      <c r="E245" t="s">
+        <v>36</v>
+      </c>
       <c r="F245" t="s">
         <v>37</v>
       </c>
@@ -14897,6 +15128,9 @@
       <c r="D246">
         <v>49</v>
       </c>
+      <c r="E246" t="s">
+        <v>36</v>
+      </c>
       <c r="F246" t="s">
         <v>37</v>
       </c>
@@ -14941,6 +15175,9 @@
       <c r="D247">
         <v>49</v>
       </c>
+      <c r="E247" t="s">
+        <v>36</v>
+      </c>
       <c r="F247" t="s">
         <v>37</v>
       </c>
@@ -14985,6 +15222,9 @@
       <c r="D248">
         <v>49</v>
       </c>
+      <c r="E248" t="s">
+        <v>36</v>
+      </c>
       <c r="F248" t="s">
         <v>37</v>
       </c>
@@ -15029,6 +15269,9 @@
       <c r="D249">
         <v>49</v>
       </c>
+      <c r="E249" t="s">
+        <v>36</v>
+      </c>
       <c r="F249" t="s">
         <v>37</v>
       </c>
@@ -15073,6 +15316,9 @@
       <c r="D250">
         <v>49</v>
       </c>
+      <c r="E250" t="s">
+        <v>36</v>
+      </c>
       <c r="F250" t="s">
         <v>37</v>
       </c>
@@ -15117,6 +15363,9 @@
       <c r="D251">
         <v>49</v>
       </c>
+      <c r="E251" t="s">
+        <v>36</v>
+      </c>
       <c r="F251" t="s">
         <v>37</v>
       </c>
@@ -15161,6 +15410,9 @@
       <c r="D252">
         <v>49</v>
       </c>
+      <c r="E252" t="s">
+        <v>36</v>
+      </c>
       <c r="F252" t="s">
         <v>37</v>
       </c>
@@ -15205,6 +15457,9 @@
       <c r="D253">
         <v>49</v>
       </c>
+      <c r="E253" t="s">
+        <v>36</v>
+      </c>
       <c r="F253" t="s">
         <v>37</v>
       </c>
@@ -15249,6 +15504,9 @@
       <c r="D254">
         <v>49</v>
       </c>
+      <c r="E254" t="s">
+        <v>36</v>
+      </c>
       <c r="F254" t="s">
         <v>37</v>
       </c>
@@ -15293,6 +15551,9 @@
       <c r="D255">
         <v>49</v>
       </c>
+      <c r="E255" t="s">
+        <v>36</v>
+      </c>
       <c r="F255" t="s">
         <v>37</v>
       </c>
@@ -15337,6 +15598,9 @@
       <c r="D256">
         <v>49</v>
       </c>
+      <c r="E256" t="s">
+        <v>36</v>
+      </c>
       <c r="F256" t="s">
         <v>37</v>
       </c>
@@ -15381,6 +15645,9 @@
       <c r="D257">
         <v>49</v>
       </c>
+      <c r="E257" t="s">
+        <v>36</v>
+      </c>
       <c r="F257" t="s">
         <v>37</v>
       </c>
@@ -15425,6 +15692,9 @@
       <c r="D258">
         <v>49</v>
       </c>
+      <c r="E258" t="s">
+        <v>36</v>
+      </c>
       <c r="F258" t="s">
         <v>37</v>
       </c>
@@ -15469,6 +15739,9 @@
       <c r="D259">
         <v>49</v>
       </c>
+      <c r="E259" t="s">
+        <v>36</v>
+      </c>
       <c r="F259" t="s">
         <v>37</v>
       </c>
@@ -15513,6 +15786,9 @@
       <c r="D260">
         <v>49</v>
       </c>
+      <c r="E260" t="s">
+        <v>36</v>
+      </c>
       <c r="F260" t="s">
         <v>37</v>
       </c>
@@ -15557,6 +15833,9 @@
       <c r="D261">
         <v>49</v>
       </c>
+      <c r="E261" t="s">
+        <v>36</v>
+      </c>
       <c r="F261" t="s">
         <v>37</v>
       </c>
@@ -15601,6 +15880,9 @@
       <c r="D262">
         <v>49</v>
       </c>
+      <c r="E262" t="s">
+        <v>36</v>
+      </c>
       <c r="F262" t="s">
         <v>37</v>
       </c>
@@ -15645,6 +15927,9 @@
       <c r="D263">
         <v>49</v>
       </c>
+      <c r="E263" t="s">
+        <v>36</v>
+      </c>
       <c r="F263" t="s">
         <v>37</v>
       </c>
@@ -15689,6 +15974,9 @@
       <c r="D264">
         <v>49</v>
       </c>
+      <c r="E264" t="s">
+        <v>36</v>
+      </c>
       <c r="F264" t="s">
         <v>37</v>
       </c>
@@ -15733,6 +16021,9 @@
       <c r="D265">
         <v>50</v>
       </c>
+      <c r="E265" t="s">
+        <v>36</v>
+      </c>
       <c r="F265" t="s">
         <v>37</v>
       </c>
@@ -15777,6 +16068,9 @@
       <c r="D266">
         <v>50</v>
       </c>
+      <c r="E266" t="s">
+        <v>36</v>
+      </c>
       <c r="F266" t="s">
         <v>37</v>
       </c>
@@ -15821,6 +16115,9 @@
       <c r="D267">
         <v>50</v>
       </c>
+      <c r="E267" t="s">
+        <v>36</v>
+      </c>
       <c r="F267" t="s">
         <v>37</v>
       </c>
@@ -15865,6 +16162,9 @@
       <c r="D268">
         <v>50</v>
       </c>
+      <c r="E268" t="s">
+        <v>36</v>
+      </c>
       <c r="F268" t="s">
         <v>37</v>
       </c>
@@ -15909,6 +16209,9 @@
       <c r="D269">
         <v>50</v>
       </c>
+      <c r="E269" t="s">
+        <v>36</v>
+      </c>
       <c r="F269" t="s">
         <v>37</v>
       </c>
@@ -15953,6 +16256,9 @@
       <c r="D270">
         <v>50</v>
       </c>
+      <c r="E270" t="s">
+        <v>36</v>
+      </c>
       <c r="F270" t="s">
         <v>37</v>
       </c>
@@ -15997,6 +16303,9 @@
       <c r="D271">
         <v>51</v>
       </c>
+      <c r="E271" t="s">
+        <v>36</v>
+      </c>
       <c r="F271" t="s">
         <v>37</v>
       </c>
@@ -16041,6 +16350,9 @@
       <c r="D272">
         <v>51</v>
       </c>
+      <c r="E272" t="s">
+        <v>36</v>
+      </c>
       <c r="F272" t="s">
         <v>37</v>
       </c>
@@ -16085,6 +16397,9 @@
       <c r="D273">
         <v>51</v>
       </c>
+      <c r="E273" t="s">
+        <v>36</v>
+      </c>
       <c r="F273" t="s">
         <v>37</v>
       </c>
@@ -16129,6 +16444,9 @@
       <c r="D274">
         <v>51</v>
       </c>
+      <c r="E274" t="s">
+        <v>36</v>
+      </c>
       <c r="F274" t="s">
         <v>37</v>
       </c>
@@ -16173,6 +16491,9 @@
       <c r="D275">
         <v>51</v>
       </c>
+      <c r="E275" t="s">
+        <v>36</v>
+      </c>
       <c r="F275" t="s">
         <v>37</v>
       </c>
@@ -16217,6 +16538,9 @@
       <c r="D276">
         <v>51</v>
       </c>
+      <c r="E276" t="s">
+        <v>36</v>
+      </c>
       <c r="F276" t="s">
         <v>37</v>
       </c>
@@ -16261,6 +16585,9 @@
       <c r="D277">
         <v>51</v>
       </c>
+      <c r="E277" t="s">
+        <v>36</v>
+      </c>
       <c r="F277" t="s">
         <v>37</v>
       </c>
@@ -16305,6 +16632,9 @@
       <c r="D278">
         <v>51</v>
       </c>
+      <c r="E278" t="s">
+        <v>36</v>
+      </c>
       <c r="F278" t="s">
         <v>37</v>
       </c>
@@ -16349,6 +16679,9 @@
       <c r="D279">
         <v>51</v>
       </c>
+      <c r="E279" t="s">
+        <v>36</v>
+      </c>
       <c r="F279" t="s">
         <v>37</v>
       </c>
@@ -16393,6 +16726,9 @@
       <c r="D280">
         <v>51</v>
       </c>
+      <c r="E280" t="s">
+        <v>36</v>
+      </c>
       <c r="F280" t="s">
         <v>37</v>
       </c>
@@ -16437,6 +16773,9 @@
       <c r="D281">
         <v>52</v>
       </c>
+      <c r="E281" t="s">
+        <v>36</v>
+      </c>
       <c r="F281" t="s">
         <v>37</v>
       </c>
@@ -16481,6 +16820,9 @@
       <c r="D282">
         <v>52</v>
       </c>
+      <c r="E282" t="s">
+        <v>36</v>
+      </c>
       <c r="F282" t="s">
         <v>37</v>
       </c>
@@ -16525,6 +16867,9 @@
       <c r="D283">
         <v>52</v>
       </c>
+      <c r="E283" t="s">
+        <v>36</v>
+      </c>
       <c r="F283" t="s">
         <v>37</v>
       </c>
@@ -16569,6 +16914,9 @@
       <c r="D284">
         <v>52</v>
       </c>
+      <c r="E284" t="s">
+        <v>36</v>
+      </c>
       <c r="F284" t="s">
         <v>37</v>
       </c>
@@ -16613,6 +16961,9 @@
       <c r="D285">
         <v>52</v>
       </c>
+      <c r="E285" t="s">
+        <v>36</v>
+      </c>
       <c r="F285" t="s">
         <v>37</v>
       </c>
@@ -16657,6 +17008,9 @@
       <c r="D286">
         <v>52</v>
       </c>
+      <c r="E286" t="s">
+        <v>36</v>
+      </c>
       <c r="F286" t="s">
         <v>37</v>
       </c>
@@ -16701,6 +17055,9 @@
       <c r="D287">
         <v>53</v>
       </c>
+      <c r="E287" t="s">
+        <v>36</v>
+      </c>
       <c r="F287" t="s">
         <v>37</v>
       </c>
@@ -16745,6 +17102,9 @@
       <c r="D288">
         <v>53</v>
       </c>
+      <c r="E288" t="s">
+        <v>36</v>
+      </c>
       <c r="F288" t="s">
         <v>37</v>
       </c>
@@ -16789,6 +17149,9 @@
       <c r="D289">
         <v>53</v>
       </c>
+      <c r="E289" t="s">
+        <v>36</v>
+      </c>
       <c r="F289" t="s">
         <v>37</v>
       </c>
@@ -16833,6 +17196,9 @@
       <c r="D290">
         <v>53</v>
       </c>
+      <c r="E290" t="s">
+        <v>36</v>
+      </c>
       <c r="F290" t="s">
         <v>37</v>
       </c>
@@ -16877,6 +17243,9 @@
       <c r="D291">
         <v>53</v>
       </c>
+      <c r="E291" t="s">
+        <v>36</v>
+      </c>
       <c r="F291" t="s">
         <v>37</v>
       </c>
@@ -16921,6 +17290,9 @@
       <c r="D292">
         <v>53</v>
       </c>
+      <c r="E292" t="s">
+        <v>36</v>
+      </c>
       <c r="F292" t="s">
         <v>37</v>
       </c>
@@ -16965,6 +17337,9 @@
       <c r="D293">
         <v>53</v>
       </c>
+      <c r="E293" t="s">
+        <v>36</v>
+      </c>
       <c r="F293" t="s">
         <v>37</v>
       </c>
@@ -17009,6 +17384,9 @@
       <c r="D294">
         <v>53</v>
       </c>
+      <c r="E294" t="s">
+        <v>36</v>
+      </c>
       <c r="F294" t="s">
         <v>37</v>
       </c>
@@ -17053,6 +17431,9 @@
       <c r="D295">
         <v>53</v>
       </c>
+      <c r="E295" t="s">
+        <v>36</v>
+      </c>
       <c r="F295" t="s">
         <v>37</v>
       </c>
@@ -17097,6 +17478,9 @@
       <c r="D296">
         <v>53</v>
       </c>
+      <c r="E296" t="s">
+        <v>36</v>
+      </c>
       <c r="F296" t="s">
         <v>37</v>
       </c>
@@ -17141,6 +17525,9 @@
       <c r="D297">
         <v>53</v>
       </c>
+      <c r="E297" t="s">
+        <v>36</v>
+      </c>
       <c r="F297" t="s">
         <v>37</v>
       </c>
@@ -17185,6 +17572,9 @@
       <c r="D298">
         <v>53</v>
       </c>
+      <c r="E298" t="s">
+        <v>36</v>
+      </c>
       <c r="F298" t="s">
         <v>37</v>
       </c>
@@ -17229,6 +17619,9 @@
       <c r="D299">
         <v>54</v>
       </c>
+      <c r="E299" t="s">
+        <v>36</v>
+      </c>
       <c r="F299" t="s">
         <v>54</v>
       </c>
@@ -17279,6 +17672,9 @@
       <c r="D300">
         <v>54</v>
       </c>
+      <c r="E300" t="s">
+        <v>36</v>
+      </c>
       <c r="F300" t="s">
         <v>54</v>
       </c>
@@ -17329,6 +17725,9 @@
       <c r="D301">
         <v>54</v>
       </c>
+      <c r="E301" t="s">
+        <v>36</v>
+      </c>
       <c r="F301" t="s">
         <v>54</v>
       </c>
@@ -17379,6 +17778,9 @@
       <c r="D302">
         <v>54</v>
       </c>
+      <c r="E302" t="s">
+        <v>36</v>
+      </c>
       <c r="F302" t="s">
         <v>54</v>
       </c>
@@ -17429,6 +17831,9 @@
       <c r="D303">
         <v>54</v>
       </c>
+      <c r="E303" t="s">
+        <v>36</v>
+      </c>
       <c r="F303" t="s">
         <v>54</v>
       </c>
@@ -17479,6 +17884,9 @@
       <c r="D304">
         <v>54</v>
       </c>
+      <c r="E304" t="s">
+        <v>36</v>
+      </c>
       <c r="F304" t="s">
         <v>54</v>
       </c>
@@ -17529,6 +17937,9 @@
       <c r="D305">
         <v>54</v>
       </c>
+      <c r="E305" t="s">
+        <v>36</v>
+      </c>
       <c r="F305" t="s">
         <v>54</v>
       </c>
@@ -17579,6 +17990,9 @@
       <c r="D306">
         <v>54</v>
       </c>
+      <c r="E306" t="s">
+        <v>36</v>
+      </c>
       <c r="F306" t="s">
         <v>54</v>
       </c>
@@ -17629,6 +18043,9 @@
       <c r="D307">
         <v>55</v>
       </c>
+      <c r="E307" t="s">
+        <v>36</v>
+      </c>
       <c r="F307" t="s">
         <v>37</v>
       </c>
@@ -17682,6 +18099,9 @@
       <c r="D308">
         <v>55</v>
       </c>
+      <c r="E308" t="s">
+        <v>36</v>
+      </c>
       <c r="F308" t="s">
         <v>37</v>
       </c>
@@ -17735,6 +18155,9 @@
       <c r="D309">
         <v>55</v>
       </c>
+      <c r="E309" t="s">
+        <v>36</v>
+      </c>
       <c r="F309" t="s">
         <v>37</v>
       </c>
@@ -17788,6 +18211,9 @@
       <c r="D310">
         <v>55</v>
       </c>
+      <c r="E310" t="s">
+        <v>36</v>
+      </c>
       <c r="F310" t="s">
         <v>37</v>
       </c>
@@ -17841,6 +18267,9 @@
       <c r="D311">
         <v>55</v>
       </c>
+      <c r="E311" t="s">
+        <v>36</v>
+      </c>
       <c r="F311" t="s">
         <v>37</v>
       </c>
@@ -17894,6 +18323,9 @@
       <c r="D312">
         <v>55</v>
       </c>
+      <c r="E312" t="s">
+        <v>36</v>
+      </c>
       <c r="F312" t="s">
         <v>37</v>
       </c>
@@ -17947,6 +18379,9 @@
       <c r="D313">
         <v>55</v>
       </c>
+      <c r="E313" t="s">
+        <v>36</v>
+      </c>
       <c r="F313" t="s">
         <v>37</v>
       </c>
@@ -18000,6 +18435,9 @@
       <c r="D314">
         <v>55</v>
       </c>
+      <c r="E314" t="s">
+        <v>36</v>
+      </c>
       <c r="F314" t="s">
         <v>37</v>
       </c>
@@ -18053,6 +18491,9 @@
       <c r="D315">
         <v>55</v>
       </c>
+      <c r="E315" t="s">
+        <v>36</v>
+      </c>
       <c r="F315" t="s">
         <v>37</v>
       </c>
@@ -18106,6 +18547,9 @@
       <c r="D316">
         <v>55</v>
       </c>
+      <c r="E316" t="s">
+        <v>36</v>
+      </c>
       <c r="F316" t="s">
         <v>37</v>
       </c>
@@ -18159,6 +18603,9 @@
       <c r="D317">
         <v>55</v>
       </c>
+      <c r="E317" t="s">
+        <v>36</v>
+      </c>
       <c r="F317" t="s">
         <v>37</v>
       </c>
@@ -18212,6 +18659,9 @@
       <c r="D318">
         <v>55</v>
       </c>
+      <c r="E318" t="s">
+        <v>36</v>
+      </c>
       <c r="F318" t="s">
         <v>37</v>
       </c>
@@ -18265,8 +18715,8 @@
       <c r="D319">
         <v>55</v>
       </c>
-      <c r="E319" s="2" t="s">
-        <v>164</v>
+      <c r="E319" t="s">
+        <v>36</v>
       </c>
       <c r="F319" t="s">
         <v>37</v>
@@ -18321,6 +18771,9 @@
       <c r="D320">
         <v>55</v>
       </c>
+      <c r="E320" t="s">
+        <v>36</v>
+      </c>
       <c r="F320" t="s">
         <v>37</v>
       </c>
@@ -18374,6 +18827,9 @@
       <c r="D321">
         <v>55</v>
       </c>
+      <c r="E321" t="s">
+        <v>36</v>
+      </c>
       <c r="F321" t="s">
         <v>37</v>
       </c>
@@ -18427,6 +18883,9 @@
       <c r="D322">
         <v>55</v>
       </c>
+      <c r="E322" t="s">
+        <v>36</v>
+      </c>
       <c r="F322" t="s">
         <v>37</v>
       </c>
@@ -18480,6 +18939,9 @@
       <c r="D323">
         <v>56</v>
       </c>
+      <c r="E323" t="s">
+        <v>36</v>
+      </c>
       <c r="F323" t="s">
         <v>54</v>
       </c>
@@ -18532,6 +18994,9 @@
       <c r="D324">
         <v>56</v>
       </c>
+      <c r="E324" t="s">
+        <v>36</v>
+      </c>
       <c r="F324" t="s">
         <v>54</v>
       </c>
@@ -18567,7 +19032,7 @@
         <v>46.018000000000001</v>
       </c>
       <c r="AI324">
-        <f t="shared" ref="AI324:AI328" si="1">200-AH324</f>
+        <f t="shared" ref="AI324:AI327" si="1">200-AH324</f>
         <v>153.982</v>
       </c>
     </row>
@@ -18584,6 +19049,9 @@
       <c r="D325">
         <v>56</v>
       </c>
+      <c r="E325" t="s">
+        <v>36</v>
+      </c>
       <c r="F325" t="s">
         <v>54</v>
       </c>
@@ -18636,6 +19104,9 @@
       <c r="D326">
         <v>56</v>
       </c>
+      <c r="E326" t="s">
+        <v>36</v>
+      </c>
       <c r="F326" t="s">
         <v>54</v>
       </c>
@@ -18688,6 +19159,9 @@
       <c r="D327">
         <v>56</v>
       </c>
+      <c r="E327" t="s">
+        <v>36</v>
+      </c>
       <c r="F327" t="s">
         <v>54</v>
       </c>
@@ -18728,6 +19202,9 @@
       </c>
     </row>
     <row r="328" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A328" t="s">
+        <v>164</v>
+      </c>
       <c r="B328" t="s">
         <v>165</v>
       </c>
@@ -18737,6 +19214,9 @@
       <c r="D328">
         <v>57</v>
       </c>
+      <c r="E328" t="s">
+        <v>43</v>
+      </c>
       <c r="F328" t="s">
         <v>54</v>
       </c>
@@ -18775,12 +19255,21 @@
       </c>
     </row>
     <row r="329" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A329" t="s">
+        <v>164</v>
+      </c>
+      <c r="B329" t="s">
+        <v>165</v>
+      </c>
       <c r="C329" t="s">
         <v>166</v>
       </c>
       <c r="D329">
         <v>57</v>
       </c>
+      <c r="E329" t="s">
+        <v>43</v>
+      </c>
       <c r="F329" t="s">
         <v>54</v>
       </c>
@@ -18813,12 +19302,21 @@
       </c>
     </row>
     <row r="330" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A330" t="s">
+        <v>164</v>
+      </c>
+      <c r="B330" t="s">
+        <v>165</v>
+      </c>
       <c r="C330" t="s">
         <v>166</v>
       </c>
       <c r="D330">
         <v>57</v>
       </c>
+      <c r="E330" t="s">
+        <v>43</v>
+      </c>
       <c r="F330" t="s">
         <v>54</v>
       </c>
@@ -18851,11 +19349,20 @@
       </c>
     </row>
     <row r="331" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A331" t="s">
+        <v>164</v>
+      </c>
+      <c r="B331" t="s">
+        <v>165</v>
+      </c>
       <c r="C331" t="s">
         <v>166</v>
       </c>
       <c r="D331">
         <v>57</v>
+      </c>
+      <c r="E331" t="s">
+        <v>43</v>
       </c>
       <c r="F331" t="s">
         <v>54</v>
@@ -18891,12 +19398,21 @@
       </c>
     </row>
     <row r="332" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A332" t="s">
+        <v>164</v>
+      </c>
+      <c r="B332" t="s">
+        <v>165</v>
+      </c>
       <c r="C332" t="s">
         <v>166</v>
       </c>
       <c r="D332">
         <v>57</v>
       </c>
+      <c r="E332" t="s">
+        <v>43</v>
+      </c>
       <c r="F332" t="s">
         <v>54</v>
       </c>
@@ -18929,11 +19445,20 @@
       </c>
     </row>
     <row r="333" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A333" t="s">
+        <v>164</v>
+      </c>
+      <c r="B333" t="s">
+        <v>165</v>
+      </c>
       <c r="C333" t="s">
         <v>166</v>
       </c>
       <c r="D333">
         <v>57</v>
+      </c>
+      <c r="E333" t="s">
+        <v>43</v>
       </c>
       <c r="F333" t="s">
         <v>54</v>
@@ -18969,11 +19494,20 @@
       </c>
     </row>
     <row r="334" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A334" t="s">
+        <v>164</v>
+      </c>
+      <c r="B334" t="s">
+        <v>165</v>
+      </c>
       <c r="C334" t="s">
         <v>163</v>
       </c>
       <c r="D334">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="E334" t="s">
+        <v>36</v>
       </c>
       <c r="F334" t="s">
         <v>54</v>
@@ -19009,11 +19543,20 @@
       </c>
     </row>
     <row r="335" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A335" t="s">
+        <v>164</v>
+      </c>
+      <c r="B335" t="s">
+        <v>165</v>
+      </c>
       <c r="C335" t="s">
         <v>163</v>
       </c>
       <c r="D335">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="E335" t="s">
+        <v>36</v>
       </c>
       <c r="F335" t="s">
         <v>54</v>
@@ -19049,11 +19592,20 @@
       </c>
     </row>
     <row r="336" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A336" t="s">
+        <v>164</v>
+      </c>
+      <c r="B336" t="s">
+        <v>165</v>
+      </c>
       <c r="C336" t="s">
         <v>163</v>
       </c>
       <c r="D336">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="E336" t="s">
+        <v>36</v>
       </c>
       <c r="F336" t="s">
         <v>54</v>
@@ -19088,12 +19640,21 @@
         <v>2.9700000000000024</v>
       </c>
     </row>
-    <row r="337" spans="3:35" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A337" t="s">
+        <v>164</v>
+      </c>
+      <c r="B337" t="s">
+        <v>165</v>
+      </c>
       <c r="C337" t="s">
         <v>163</v>
       </c>
       <c r="D337">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="E337" t="s">
+        <v>36</v>
       </c>
       <c r="F337" t="s">
         <v>54</v>
@@ -19128,12 +19689,21 @@
         <v>9.2078999999999986</v>
       </c>
     </row>
-    <row r="338" spans="3:35" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A338" t="s">
+        <v>164</v>
+      </c>
+      <c r="B338" t="s">
+        <v>165</v>
+      </c>
       <c r="C338" t="s">
         <v>163</v>
       </c>
       <c r="D338">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="E338" t="s">
+        <v>36</v>
       </c>
       <c r="F338" t="s">
         <v>54</v>
@@ -19168,12 +19738,21 @@
         <v>1.929000000000002</v>
       </c>
     </row>
-    <row r="339" spans="3:35" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A339" t="s">
+        <v>164</v>
+      </c>
+      <c r="B339" t="s">
+        <v>165</v>
+      </c>
       <c r="C339" t="s">
         <v>163</v>
       </c>
       <c r="D339">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="E339" t="s">
+        <v>36</v>
       </c>
       <c r="F339" t="s">
         <v>54</v>

</xml_diff>